<commit_message>
end of day3 with files to clean
</commit_message>
<xml_diff>
--- a/day3/02_03.xlsx
+++ b/day3/02_03.xlsx
@@ -24,12 +24,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Sales Dollars</t>
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Sales Forecast</t>
+  </si>
+  <si>
+    <t>Squared Error</t>
+  </si>
+  <si>
+    <t>RMSE</t>
+  </si>
+  <si>
+    <t>Mean square error</t>
+  </si>
+  <si>
+    <t>Excel pred</t>
   </si>
 </sst>
 </file>
@@ -40,7 +64,7 @@
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,13 +79,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -77,11 +114,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Monétaire" xfId="1" builtinId="4"/>
@@ -98,6 +137,1080 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Sales</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" baseline="0"/>
+              <a:t> forecast</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10660420928134376"/>
+          <c:y val="0.22137346669826446"/>
+          <c:w val="0.85437483857896912"/>
+          <c:h val="0.68636865221172327"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Data Analysis Tool'!$B$1:$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Sales Dollars</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v> $941 </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Data Analysis Tool'!$B$3:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #\ ##0_);_("$"* \(#\ ##0\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2557</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4987</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1658</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1494</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4857</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9799</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3949</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7489</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6495</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4797</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1401</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>756</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4457</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6478</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7174</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6302</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>991</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CF91-4372-91DC-0F3FD50D4258}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Data Analysis Tool'!$C$1:$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Sales Forecast</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Data Analysis Tool'!$C$3:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #\ ##0_);_("$"* \(#\ ##0\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>941</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1314.4499999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1749.3424999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2882.5226249999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2453.9397062499997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2117.9608090624997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3076.6245258906247</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5429.4559418289055</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4911.2963621887884</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5813.4926354227127</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6052.0202130247635</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5612.7631384660963</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4138.6460400029628</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2954.7199260019261</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3480.5179519012518</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4529.6366687358131</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5455.1638346782784</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5751.5564925408808</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CF91-4372-91DC-0F3FD50D4258}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1028223311"/>
+        <c:axId val="1028229135"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1028223311"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1028229135"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1028229135"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(&quot;$&quot;* #\ ##0_);_(&quot;$&quot;* \(#\ ##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1028223311"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>705970</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>603006</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -397,18 +1510,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" customWidth="1"/>
     <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -419,6 +1534,30 @@
       <c r="B1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -427,6 +1566,9 @@
       <c r="B2" s="2">
         <v>941</v>
       </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -435,7 +1577,26 @@
       <c r="B3" s="2">
         <v>2008</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="C3">
+        <f>941</f>
+        <v>941</v>
+      </c>
+      <c r="D3" s="3">
+        <f>B3-C3</f>
+        <v>1067</v>
+      </c>
+      <c r="E3" s="3">
+        <f>D3^2</f>
+        <v>1138489</v>
+      </c>
+      <c r="F3" s="3">
+        <f>AVERAGE(E3:E20)</f>
+        <v>8330553.3949629283</v>
+      </c>
+      <c r="G3">
+        <f>SQRT(F3)</f>
+        <v>2886.2698063353205</v>
+      </c>
       <c r="R3" s="3"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -445,6 +1606,18 @@
       <c r="B4" s="2">
         <v>2557</v>
       </c>
+      <c r="C4" s="3">
+        <f>$B3-$L$1*D3</f>
+        <v>1314.4499999999998</v>
+      </c>
+      <c r="D4" s="3">
+        <f>B4-C4</f>
+        <v>1242.5500000000002</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" ref="E4:E20" si="0">D4^2</f>
+        <v>1543930.5025000004</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -453,6 +1626,18 @@
       <c r="B5" s="2">
         <v>4987</v>
       </c>
+      <c r="C5" s="3">
+        <f>$B4-$L$1*D4</f>
+        <v>1749.3424999999997</v>
+      </c>
+      <c r="D5" s="3">
+        <f>B5-C5</f>
+        <v>3237.6575000000003</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>10482426.087306252</v>
+      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -461,6 +1646,18 @@
       <c r="B6" s="2">
         <v>1658</v>
       </c>
+      <c r="C6" s="3">
+        <f>$B5-$L$1*D5</f>
+        <v>2882.5226249999996</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" ref="D4:D20" si="1">B6-C6</f>
+        <v>-1224.5226249999996</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
+        <v>1499455.6591368897</v>
+      </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -469,6 +1666,18 @@
       <c r="B7" s="2">
         <v>1494</v>
       </c>
+      <c r="C7" s="3">
+        <f>$B6-$L$1*D6</f>
+        <v>2453.9397062499997</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="1"/>
+        <v>-959.93970624999974</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>921484.23963533575</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -477,6 +1686,18 @@
       <c r="B8" s="2">
         <v>4857</v>
       </c>
+      <c r="C8" s="3">
+        <f>$B7-$L$1*D7</f>
+        <v>2117.9608090624997</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="1"/>
+        <v>2739.0391909375003</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>7502335.689491556</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -485,6 +1706,18 @@
       <c r="B9" s="2">
         <v>9799</v>
       </c>
+      <c r="C9" s="3">
+        <f>$B8-$L$1*D8</f>
+        <v>3076.6245258906247</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="1"/>
+        <v>6722.3754741093753</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>45190332.014907248</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -493,6 +1726,18 @@
       <c r="B10" s="2">
         <v>3949</v>
       </c>
+      <c r="C10" s="3">
+        <f>$B9-$L$1*D9</f>
+        <v>5429.4559418289055</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="1"/>
+        <v>-1480.4559418289055</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
+        <v>2191749.7956965114</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -501,6 +1746,18 @@
       <c r="B11" s="2">
         <v>7489</v>
       </c>
+      <c r="C11" s="3">
+        <f>$B10-$L$1*D10</f>
+        <v>4911.2963621887884</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="1"/>
+        <v>2577.7036378112116</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>6644556.0443851538</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -509,6 +1766,18 @@
       <c r="B12" s="2">
         <v>6495</v>
       </c>
+      <c r="C12" s="3">
+        <f>$B11-$L$1*D11</f>
+        <v>5813.4926354227127</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="1"/>
+        <v>681.50736457728726</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>464452.28797307954</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -517,6 +1786,18 @@
       <c r="B13" s="2">
         <v>4797</v>
       </c>
+      <c r="C13" s="3">
+        <f>$B12-$L$1*D12</f>
+        <v>6052.0202130247635</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="1"/>
+        <v>-1255.0202130247635</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
+        <v>1575075.7351007229</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -525,6 +1806,18 @@
       <c r="B14" s="2">
         <v>1401</v>
       </c>
+      <c r="C14" s="3">
+        <f>$B13-$L$1*D13</f>
+        <v>5612.7631384660963</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="1"/>
+        <v>-4211.7631384660963</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
+        <v>17738948.734541781</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -533,6 +1826,18 @@
       <c r="B15" s="2">
         <v>756</v>
       </c>
+      <c r="C15" s="3">
+        <f>$B14-$L$1*D14</f>
+        <v>4138.6460400029628</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="1"/>
+        <v>-3382.6460400029628</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="0"/>
+        <v>11442294.231947726</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -541,40 +1846,160 @@
       <c r="B16" s="2">
         <v>4457</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="3">
+        <f>$B15-$L$1*D15</f>
+        <v>2954.7199260019261</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="1"/>
+        <v>1502.2800739980739</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="0"/>
+        <v>2256845.4207316586</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>42902</v>
       </c>
       <c r="B17" s="2">
         <v>6478</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="3">
+        <f>$B16-$L$1*D16</f>
+        <v>3480.5179519012518</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="1"/>
+        <v>2997.4820480987482</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="0"/>
+        <v>8984898.6286742669</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>42903</v>
       </c>
       <c r="B18" s="2">
         <v>7174</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="3">
+        <f>$B17-$L$1*D17</f>
+        <v>4529.6366687358131</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="1"/>
+        <v>2644.3633312641869</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="0"/>
+        <v>6992657.4277346274</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>42904</v>
       </c>
       <c r="B19" s="2">
         <v>6302</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="3">
+        <f>$B18-$L$1*D18</f>
+        <v>5455.1638346782784</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="1"/>
+        <v>846.83616532172164</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="0"/>
+        <v>717131.4908967982</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>42905</v>
       </c>
       <c r="B20" s="2">
         <v>991</v>
       </c>
+      <c r="C20" s="3">
+        <f>$B19-$L$1*D19</f>
+        <v>5751.5564925408808</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="1"/>
+        <v>-4760.5564925408808</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="0"/>
+        <v>22662898.118673135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>0.1</v>
+      </c>
+      <c r="E25">
+        <v>2983.3875556480061</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>0.2</v>
+      </c>
+      <c r="E26">
+        <v>2957.9371228714263</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>0.4</v>
+      </c>
+      <c r="E27">
+        <v>2920.1950666153557</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>0.5</v>
+      </c>
+      <c r="E28">
+        <v>2903.3893328056556</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D29" s="4">
+        <v>0.65</v>
+      </c>
+      <c r="E29" s="5">
+        <v>2886.2698063353205</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>0.7</v>
+      </c>
+      <c r="E30">
+        <v>2888.4557149529992</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="D25:E30">
+    <sortCondition ref="D25"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>